<commit_message>
fix : conrrection de l'export du zip
</commit_message>
<xml_diff>
--- a/src/test/resources/test_error.xlsx
+++ b/src/test/resources/test_error.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">Numéro du groupe </t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>OK</t>
-  </si>
-  <si>
-    <t>Théo Jasmin</t>
   </si>
   <si>
     <t>3 rue des Vignes</t>
@@ -506,9 +503,9 @@
   </sheetPr>
   <dimension ref="A1:AF735"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -603,20 +600,18 @@
         <v>11</v>
       </c>
       <c r="B2" s="11"/>
-      <c r="C2" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="C2" s="11"/>
       <c r="D2" s="12">
         <v>43863</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="11" t="s">
         <v>17</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>18</v>
       </c>
       <c r="H2" s="11">
         <v>2000</v>

</xml_diff>